<commit_message>
QuestionAndAnswer: some csproj/sln administration.
</commit_message>
<xml_diff>
--- a/Presentation/QuestionAndAnswer.Import.WinForms/IO Files/DutchToPolish.xlsx
+++ b/Presentation/QuestionAndAnswer.Import.WinForms/IO Files/DutchToPolish.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\JJs Software\JJ TFS\Presentation\QuestionAndAnswer.Import.WinForms\IO Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA0D01F-A627-44BC-B037-D8F3B4B3AC3F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6D1F35-B655-4A42-8969-97DDAF4803CD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20633" windowHeight="7791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="431">
   <si>
     <t>CultureCodeA</t>
   </si>
@@ -1333,6 +1333,12 @@
   </si>
   <si>
     <t>ona</t>
+  </si>
+  <si>
+    <t>lijst</t>
+  </si>
+  <si>
+    <t>lista</t>
   </si>
 </sst>
 </file>
@@ -2186,11 +2192,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F169"/>
+  <dimension ref="A1:F170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
+      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B170" sqref="B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4968,6 +4974,20 @@
         <v>428</v>
       </c>
     </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>5</v>
+      </c>
+      <c r="B170" t="s">
+        <v>429</v>
+      </c>
+      <c r="C170" t="s">
+        <v>7</v>
+      </c>
+      <c r="D170" t="s">
+        <v>430</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:E164">
     <sortCondition ref="B2:B164"/>

</xml_diff>